<commit_message>
change position of calculating F(x)
git-svn-id: svn+ssh://arith-c.math.se.tmu.ac.jp/var/svn/repos/abst/trunk@202 ee56edd8-5187-8145-a53a-5b855f78f1fc
</commit_message>
<xml_diff>
--- a/doc/mpqs処理速度.xlsx
+++ b/doc/mpqs処理速度.xlsx
@@ -619,7 +619,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -684,7 +684,7 @@
         <v>0.109</v>
       </c>
       <c r="G2" s="7">
-        <v>7.8E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>27</v>
@@ -713,7 +713,7 @@
         <v>0.79600000000000004</v>
       </c>
       <c r="G3" s="7">
-        <v>0.436</v>
+        <v>0.374</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>6</v>
@@ -742,7 +742,7 @@
         <v>3.6190000000000002</v>
       </c>
       <c r="G4" s="7">
-        <v>2.823</v>
+        <v>2.5430000000000001</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>11</v>
@@ -771,7 +771,7 @@
         <v>40.591000000000001</v>
       </c>
       <c r="G5" s="7">
-        <v>7.55</v>
+        <v>7.1139999999999999</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>15</v>
@@ -798,7 +798,7 @@
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7">
-        <v>193.41</v>
+        <v>182.34899999999999</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>20</v>

</xml_diff>